<commit_message>
update to comply with new components
</commit_message>
<xml_diff>
--- a/heat_sens/docs/heat_values.xlsx
+++ b/heat_sens/docs/heat_values.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="8595" windowHeight="9795"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="8595" windowHeight="9795" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>RAW values</t>
   </si>
@@ -29,6 +29,15 @@
   <si>
     <t>max</t>
   </si>
+  <si>
+    <t>2 step linerar interpolation</t>
+  </si>
+  <si>
+    <t>first X</t>
+  </si>
+  <si>
+    <t>then Y</t>
+  </si>
 </sst>
 </file>
 
@@ -37,7 +46,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -47,6 +56,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -89,9 +105,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -765,26 +783,26 @@
           </c:val>
         </c:ser>
         <c:bandFmts/>
-        <c:axId val="217661440"/>
-        <c:axId val="217662976"/>
-        <c:axId val="194293248"/>
+        <c:axId val="184465664"/>
+        <c:axId val="184471552"/>
+        <c:axId val="184459264"/>
       </c:surfaceChart>
       <c:catAx>
-        <c:axId val="217661440"/>
+        <c:axId val="184465664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="217662976"/>
+        <c:crossAx val="184471552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="217662976"/>
+        <c:axId val="184471552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="30"/>
@@ -794,20 +812,20 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ " sourceLinked="1"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="217661440"/>
+        <c:crossAx val="184465664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
         <c:minorUnit val="0.2"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="194293248"/>
+        <c:axId val="184459264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="217662976"/>
+        <c:crossAx val="184471552"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
     </c:plotArea>
@@ -829,7 +847,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1498,26 +1516,26 @@
           </c:val>
         </c:ser>
         <c:bandFmts/>
-        <c:axId val="219953408"/>
-        <c:axId val="220090368"/>
-        <c:axId val="220071680"/>
+        <c:axId val="182622464"/>
+        <c:axId val="182628352"/>
+        <c:axId val="182585984"/>
       </c:surface3DChart>
       <c:catAx>
-        <c:axId val="219953408"/>
+        <c:axId val="182622464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="220090368"/>
+        <c:crossAx val="182628352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="220090368"/>
+        <c:axId val="182628352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="30"/>
@@ -1527,20 +1545,20 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ " sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="219953408"/>
+        <c:crossAx val="182622464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
         <c:minorUnit val="0.2"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="220071680"/>
+        <c:axId val="182585984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="220090368"/>
+        <c:crossAx val="182628352"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
     </c:plotArea>
@@ -1562,7 +1580,961 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="nl-BE"/>
+  <c:style val="4"/>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:view3D>
+      <c:rotX val="90"/>
+      <c:rotY val="0"/>
+      <c:perspective val="0"/>
+    </c:view3D>
+    <c:plotArea>
+      <c:layout/>
+      <c:surfaceChart>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$13:$P$13</c:f>
+              <c:numCache>
+                <c:formatCode>_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * "-"??_ ;_ @_ </c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>22.75</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22.375</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>22.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>21.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>21.375</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>21.25</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>20.875</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>20.875</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>21.25</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>21.25</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>21.25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$14:$P$14</c:f>
+              <c:numCache>
+                <c:formatCode>_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * "-"??_ ;_ @_ </c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>22.75</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22.375</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22.0625</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>22.125</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>21.8125</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>21.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>21.3125</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>21.125</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>20.9375</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20.75</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>21.0625</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>21.375</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>21.375</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>21.375</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$15:$P$15</c:f>
+              <c:numCache>
+                <c:formatCode>_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * "-"??_ ;_ @_ </c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>22.75</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22.375</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21.875</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>21.75</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>21.625</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>21.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>21.25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>21.25</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>21.5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>21.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>21.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$16:$P$16</c:f>
+              <c:numCache>
+                <c:formatCode>_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * "-"??_ ;_ @_ </c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>22.625</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22.1875</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21.8125</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>21.875</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>21.875</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>21.875</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>21.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>21.125</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>21.0625</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>21.3125</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>21.625</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>21.625</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>21.625</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$17:$P$17</c:f>
+              <c:numCache>
+                <c:formatCode>_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * "-"??_ ;_ @_ </c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>22.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21.75</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22.125</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>22.25</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>21.75</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>21.25</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>21.125</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>21.375</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>21.75</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>21.75</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>21.75</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$18:$P$18</c:f>
+              <c:numCache>
+                <c:formatCode>_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * "-"??_ ;_ @_ </c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>22.125</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21.875</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>22.125</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22.4375</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>22.75</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>22.6875</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>22.625</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>22.3125</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>22.0625</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>22.125</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>22.1875</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>22.25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$19:$P$19</c:f>
+              <c:numCache>
+                <c:formatCode>_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * "-"??_ ;_ @_ </c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>21.75</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>22.25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22.75</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>23.25</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>23.625</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>23.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>22.75</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>22.5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>22.625</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>22.75</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$20:$P$20</c:f>
+              <c:numCache>
+                <c:formatCode>_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * "-"??_ ;_ @_ </c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>21.75</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21.8125</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21.875</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21.9375</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>23.625</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>25.25</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>25.8125</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>26.375</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>26.25</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>26.125</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>25.875</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>26.125</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$21:$P$21</c:f>
+              <c:numCache>
+                <c:formatCode>_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * "-"??_ ;_ @_ </c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>21.75</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21.625</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21.625</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>21.75</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>27.25</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>28.75</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>29.25</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>29.25</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>29.25</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>29.375</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>29.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$22:$P$22</c:f>
+              <c:numCache>
+                <c:formatCode>_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * "-"??_ ;_ @_ </c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>21.875</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21.5625</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21.375</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>21.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>23.1875</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24.875</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>25.6875</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>26.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>26.75</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>27.1875</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>27.375</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>27.25</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>27.125</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="10"/>
+          <c:order val="10"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$23:$P$23</c:f>
+              <c:numCache>
+                <c:formatCode>_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * "-"??_ ;_ @_ </c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21.125</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>21.25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>21.875</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>22.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>23.375</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>24.25</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>24.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>24.75</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>25.125</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>25.5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>25.125</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>24.75</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="11"/>
+          <c:order val="11"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$24:$P$24</c:f>
+              <c:numCache>
+                <c:formatCode>_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * "-"??_ ;_ @_ </c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>21.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21.375</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>21.25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>21.6875</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>22.125</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>22.625</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>23.125</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>23.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>23.875</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>24.1875</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>24.5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>24.3125</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>24.125</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="12"/>
+          <c:order val="12"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$25:$P$25</c:f>
+              <c:numCache>
+                <c:formatCode>_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * "-"??_ ;_ @_ </c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21.375</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>21.25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>21.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>21.75</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>21.875</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>22.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>23.25</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>23.5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>23.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>23.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="13"/>
+          <c:order val="13"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$26:$P$26</c:f>
+              <c:numCache>
+                <c:formatCode>_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * "-"??_ ;_ @_ </c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>21.125</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21.375</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21.375</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>21.375</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>21.6875</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>22.0625</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>22.125</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>22.375</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>22.625</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>22.9375</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>23.25</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>23.3125</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>23.375</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="14"/>
+          <c:order val="14"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$27:$P$27</c:f>
+              <c:numCache>
+                <c:formatCode>_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * "-"??_ ;_ @_ </c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>21.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21.375</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>21.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>21.875</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>22.25</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>22.25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>22.25</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>22.25</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>22.25</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>22.625</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>23.125</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>23.25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:bandFmts/>
+        <c:axId val="61305216"/>
+        <c:axId val="61307904"/>
+        <c:axId val="61763584"/>
+      </c:surfaceChart>
+      <c:catAx>
+        <c:axId val="61305216"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="61307904"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="61307904"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="30"/>
+          <c:min val="20"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ " sourceLinked="1"/>
+        <c:tickLblPos val="none"/>
+        <c:crossAx val="61305216"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1"/>
+        <c:minorUnit val="0.2"/>
+      </c:valAx>
+      <c:serAx>
+        <c:axId val="61763584"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="61307904"/>
+        <c:crosses val="autoZero"/>
+      </c:serAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="nl-BE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1625,6 +2597,41 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>133349</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1920,8 +2927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A5:P69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+    <sheetView topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6:M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2027,7 +3034,7 @@
         <v>88</v>
       </c>
       <c r="C7">
-        <f t="shared" ref="C7:C70" si="1">B7/4</f>
+        <f t="shared" ref="C7:C69" si="1">B7/4</f>
         <v>22</v>
       </c>
       <c r="E7">
@@ -2075,7 +3082,7 @@
     </row>
     <row r="8" spans="1:16">
       <c r="A8">
-        <f t="shared" ref="A8:A70" si="3">A7+1</f>
+        <f t="shared" ref="A8:A69" si="3">A7+1</f>
         <v>2</v>
       </c>
       <c r="B8">
@@ -3097,13 +4104,1356 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:Q33"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="11.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17">
+      <c r="B1" s="2">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2">
+        <v>6</v>
+      </c>
+      <c r="I1" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
+      <c r="A2" s="2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2">
+        <v>22.75</v>
+      </c>
+      <c r="C2" s="2">
+        <v>22</v>
+      </c>
+      <c r="D2" s="2">
+        <v>22.5</v>
+      </c>
+      <c r="E2" s="2">
+        <v>21.5</v>
+      </c>
+      <c r="F2" s="2">
+        <v>21.25</v>
+      </c>
+      <c r="G2" s="2">
+        <v>20.5</v>
+      </c>
+      <c r="H2" s="2">
+        <v>21.25</v>
+      </c>
+      <c r="I2" s="2">
+        <v>21.25</v>
+      </c>
+      <c r="K2" s="2">
+        <f>MIN(B2:I9)</f>
+        <v>20.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
+        <v>22.75</v>
+      </c>
+      <c r="C3" s="2">
+        <v>22</v>
+      </c>
+      <c r="D3" s="2">
+        <v>21.75</v>
+      </c>
+      <c r="E3" s="2">
+        <v>21.5</v>
+      </c>
+      <c r="F3" s="2">
+        <v>21</v>
+      </c>
+      <c r="G3" s="2">
+        <v>21</v>
+      </c>
+      <c r="H3" s="2">
+        <v>21.5</v>
+      </c>
+      <c r="I3" s="2">
+        <v>21.5</v>
+      </c>
+      <c r="K3" s="2">
+        <f>MAX(B2:I9)</f>
+        <v>29.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2">
+        <v>22.5</v>
+      </c>
+      <c r="C4" s="2">
+        <v>21.5</v>
+      </c>
+      <c r="D4" s="2">
+        <v>22</v>
+      </c>
+      <c r="E4" s="2">
+        <v>22.25</v>
+      </c>
+      <c r="F4" s="2">
+        <v>21.25</v>
+      </c>
+      <c r="G4" s="2">
+        <v>21</v>
+      </c>
+      <c r="H4" s="2">
+        <v>21.75</v>
+      </c>
+      <c r="I4" s="2">
+        <v>21.75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2">
+        <v>21.75</v>
+      </c>
+      <c r="C5" s="2">
+        <v>22.25</v>
+      </c>
+      <c r="D5" s="2">
+        <v>22.25</v>
+      </c>
+      <c r="E5" s="2">
+        <v>23.25</v>
+      </c>
+      <c r="F5" s="2">
+        <v>24</v>
+      </c>
+      <c r="G5" s="2">
+        <v>23</v>
+      </c>
+      <c r="H5" s="2">
+        <v>22.5</v>
+      </c>
+      <c r="I5" s="2">
+        <v>22.75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2">
+        <v>21.75</v>
+      </c>
+      <c r="C6" s="2">
+        <v>21.5</v>
+      </c>
+      <c r="D6" s="2">
+        <v>21.75</v>
+      </c>
+      <c r="E6" s="2">
+        <v>27.25</v>
+      </c>
+      <c r="F6" s="2">
+        <v>28.75</v>
+      </c>
+      <c r="G6" s="2">
+        <v>29.25</v>
+      </c>
+      <c r="H6" s="2">
+        <v>29.25</v>
+      </c>
+      <c r="I6" s="2">
+        <v>29.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
+      <c r="A7" s="2">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2">
+        <v>22</v>
+      </c>
+      <c r="C7" s="2">
+        <v>21</v>
+      </c>
+      <c r="D7" s="2">
+        <v>21.25</v>
+      </c>
+      <c r="E7" s="2">
+        <v>22.5</v>
+      </c>
+      <c r="F7" s="2">
+        <v>24.25</v>
+      </c>
+      <c r="G7" s="2">
+        <v>24.75</v>
+      </c>
+      <c r="H7" s="2">
+        <v>25.5</v>
+      </c>
+      <c r="I7" s="2">
+        <v>24.75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
+      <c r="A8" s="2">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2">
+        <v>21</v>
+      </c>
+      <c r="C8" s="2">
+        <v>21.5</v>
+      </c>
+      <c r="D8" s="2">
+        <v>21.25</v>
+      </c>
+      <c r="E8" s="2">
+        <v>21.75</v>
+      </c>
+      <c r="F8" s="2">
+        <v>22</v>
+      </c>
+      <c r="G8" s="2">
+        <v>23</v>
+      </c>
+      <c r="H8" s="2">
+        <v>23.5</v>
+      </c>
+      <c r="I8" s="2">
+        <v>23.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
+      <c r="A9" s="2">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2">
+        <v>21.25</v>
+      </c>
+      <c r="C9" s="2">
+        <v>21.25</v>
+      </c>
+      <c r="D9" s="2">
+        <v>21.5</v>
+      </c>
+      <c r="E9" s="2">
+        <v>22.25</v>
+      </c>
+      <c r="F9" s="2">
+        <v>22.25</v>
+      </c>
+      <c r="G9" s="2">
+        <v>22.25</v>
+      </c>
+      <c r="H9" s="2">
+        <v>23</v>
+      </c>
+      <c r="I9" s="2">
+        <v>23.25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
+      <c r="B12" s="2">
+        <v>0</v>
+      </c>
+      <c r="C12" s="2">
+        <v>1</v>
+      </c>
+      <c r="D12" s="2">
+        <v>2</v>
+      </c>
+      <c r="E12" s="2">
+        <v>3</v>
+      </c>
+      <c r="F12" s="2">
+        <v>4</v>
+      </c>
+      <c r="G12" s="2">
+        <v>5</v>
+      </c>
+      <c r="H12" s="2">
+        <v>6</v>
+      </c>
+      <c r="I12" s="2">
+        <v>7</v>
+      </c>
+      <c r="J12" s="2">
+        <v>8</v>
+      </c>
+      <c r="K12" s="2">
+        <v>9</v>
+      </c>
+      <c r="L12" s="2">
+        <v>10</v>
+      </c>
+      <c r="M12" s="2">
+        <v>11</v>
+      </c>
+      <c r="N12" s="2">
+        <v>12</v>
+      </c>
+      <c r="O12" s="2">
+        <v>13</v>
+      </c>
+      <c r="P12" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
+      <c r="A13" s="2">
+        <v>0</v>
+      </c>
+      <c r="B13" s="3">
+        <f ca="1">OFFSET($B$2,$A13/2,B$12/2)</f>
+        <v>22.75</v>
+      </c>
+      <c r="C13" s="3">
+        <f ca="1">B13/2+D13/2</f>
+        <v>22.375</v>
+      </c>
+      <c r="D13" s="3">
+        <f t="shared" ref="C13:Q13" ca="1" si="0">OFFSET($B$2,$A13/2,D$12/2)</f>
+        <v>22</v>
+      </c>
+      <c r="E13" s="3">
+        <f ca="1">D13/2+F13/2</f>
+        <v>22.25</v>
+      </c>
+      <c r="F13" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>22.5</v>
+      </c>
+      <c r="G13" s="3">
+        <f ca="1">F13/2+H13/2</f>
+        <v>22</v>
+      </c>
+      <c r="H13" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>21.5</v>
+      </c>
+      <c r="I13" s="3">
+        <f ca="1">H13/2+J13/2</f>
+        <v>21.375</v>
+      </c>
+      <c r="J13" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>21.25</v>
+      </c>
+      <c r="K13" s="3">
+        <f ca="1">J13/2+L13/2</f>
+        <v>20.875</v>
+      </c>
+      <c r="L13" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>20.5</v>
+      </c>
+      <c r="M13" s="3">
+        <f ca="1">L13/2+N13/2</f>
+        <v>20.875</v>
+      </c>
+      <c r="N13" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>21.25</v>
+      </c>
+      <c r="O13" s="3">
+        <f ca="1">N13/2+P13/2</f>
+        <v>21.25</v>
+      </c>
+      <c r="P13" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>21.25</v>
+      </c>
+      <c r="Q13" s="3"/>
+    </row>
+    <row r="14" spans="1:17">
+      <c r="A14" s="2">
+        <v>1</v>
+      </c>
+      <c r="B14" s="3">
+        <f ca="1">B13/2+B15/2</f>
+        <v>22.75</v>
+      </c>
+      <c r="C14" s="3">
+        <f t="shared" ref="C14:P14" ca="1" si="1">C13/2+C15/2</f>
+        <v>22.375</v>
+      </c>
+      <c r="D14" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="E14" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>22.0625</v>
+      </c>
+      <c r="F14" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>22.125</v>
+      </c>
+      <c r="G14" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>21.8125</v>
+      </c>
+      <c r="H14" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>21.5</v>
+      </c>
+      <c r="I14" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>21.3125</v>
+      </c>
+      <c r="J14" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>21.125</v>
+      </c>
+      <c r="K14" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>20.9375</v>
+      </c>
+      <c r="L14" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>20.75</v>
+      </c>
+      <c r="M14" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>21.0625</v>
+      </c>
+      <c r="N14" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>21.375</v>
+      </c>
+      <c r="O14" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>21.375</v>
+      </c>
+      <c r="P14" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>21.375</v>
+      </c>
+      <c r="Q14" s="3"/>
+    </row>
+    <row r="15" spans="1:17">
+      <c r="A15" s="2">
+        <v>2</v>
+      </c>
+      <c r="B15" s="3">
+        <f t="shared" ref="B14:Q28" ca="1" si="2">OFFSET($B$2,$A15/2,B$12/2)</f>
+        <v>22.75</v>
+      </c>
+      <c r="C15" s="3">
+        <f t="shared" ref="C15:E15" ca="1" si="3">B15/2+D15/2</f>
+        <v>22.375</v>
+      </c>
+      <c r="D15" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="E15" s="3">
+        <f t="shared" ca="1" si="3"/>
+        <v>21.875</v>
+      </c>
+      <c r="F15" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>21.75</v>
+      </c>
+      <c r="G15" s="3">
+        <f t="shared" ref="G15" ca="1" si="4">F15/2+H15/2</f>
+        <v>21.625</v>
+      </c>
+      <c r="H15" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>21.5</v>
+      </c>
+      <c r="I15" s="3">
+        <f t="shared" ref="I15" ca="1" si="5">H15/2+J15/2</f>
+        <v>21.25</v>
+      </c>
+      <c r="J15" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="K15" s="3">
+        <f t="shared" ref="K15" ca="1" si="6">J15/2+L15/2</f>
+        <v>21</v>
+      </c>
+      <c r="L15" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="M15" s="3">
+        <f t="shared" ref="M15" ca="1" si="7">L15/2+N15/2</f>
+        <v>21.25</v>
+      </c>
+      <c r="N15" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>21.5</v>
+      </c>
+      <c r="O15" s="3">
+        <f t="shared" ref="O15" ca="1" si="8">N15/2+P15/2</f>
+        <v>21.5</v>
+      </c>
+      <c r="P15" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>21.5</v>
+      </c>
+      <c r="Q15" s="3"/>
+    </row>
+    <row r="16" spans="1:17">
+      <c r="A16" s="2">
+        <v>3</v>
+      </c>
+      <c r="B16" s="3">
+        <f ca="1">B15/2+B17/2</f>
+        <v>22.625</v>
+      </c>
+      <c r="C16" s="3">
+        <f t="shared" ref="C16" ca="1" si="9">C15/2+C17/2</f>
+        <v>22.1875</v>
+      </c>
+      <c r="D16" s="3">
+        <f t="shared" ref="D16" ca="1" si="10">D15/2+D17/2</f>
+        <v>21.75</v>
+      </c>
+      <c r="E16" s="3">
+        <f t="shared" ref="E16" ca="1" si="11">E15/2+E17/2</f>
+        <v>21.8125</v>
+      </c>
+      <c r="F16" s="3">
+        <f t="shared" ref="F16" ca="1" si="12">F15/2+F17/2</f>
+        <v>21.875</v>
+      </c>
+      <c r="G16" s="3">
+        <f t="shared" ref="G16" ca="1" si="13">G15/2+G17/2</f>
+        <v>21.875</v>
+      </c>
+      <c r="H16" s="3">
+        <f t="shared" ref="H16" ca="1" si="14">H15/2+H17/2</f>
+        <v>21.875</v>
+      </c>
+      <c r="I16" s="3">
+        <f t="shared" ref="I16" ca="1" si="15">I15/2+I17/2</f>
+        <v>21.5</v>
+      </c>
+      <c r="J16" s="3">
+        <f t="shared" ref="J16" ca="1" si="16">J15/2+J17/2</f>
+        <v>21.125</v>
+      </c>
+      <c r="K16" s="3">
+        <f t="shared" ref="K16" ca="1" si="17">K15/2+K17/2</f>
+        <v>21.0625</v>
+      </c>
+      <c r="L16" s="3">
+        <f t="shared" ref="L16" ca="1" si="18">L15/2+L17/2</f>
+        <v>21</v>
+      </c>
+      <c r="M16" s="3">
+        <f t="shared" ref="M16" ca="1" si="19">M15/2+M17/2</f>
+        <v>21.3125</v>
+      </c>
+      <c r="N16" s="3">
+        <f t="shared" ref="N16" ca="1" si="20">N15/2+N17/2</f>
+        <v>21.625</v>
+      </c>
+      <c r="O16" s="3">
+        <f t="shared" ref="O16" ca="1" si="21">O15/2+O17/2</f>
+        <v>21.625</v>
+      </c>
+      <c r="P16" s="3">
+        <f t="shared" ref="P16" ca="1" si="22">P15/2+P17/2</f>
+        <v>21.625</v>
+      </c>
+      <c r="Q16" s="3"/>
+    </row>
+    <row r="17" spans="1:17">
+      <c r="A17" s="2">
+        <v>4</v>
+      </c>
+      <c r="B17" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>22.5</v>
+      </c>
+      <c r="C17" s="3">
+        <f t="shared" ref="C17:E17" ca="1" si="23">B17/2+D17/2</f>
+        <v>22</v>
+      </c>
+      <c r="D17" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>21.5</v>
+      </c>
+      <c r="E17" s="3">
+        <f t="shared" ca="1" si="23"/>
+        <v>21.75</v>
+      </c>
+      <c r="F17" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="G17" s="3">
+        <f t="shared" ref="G17" ca="1" si="24">F17/2+H17/2</f>
+        <v>22.125</v>
+      </c>
+      <c r="H17" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>22.25</v>
+      </c>
+      <c r="I17" s="3">
+        <f t="shared" ref="I17" ca="1" si="25">H17/2+J17/2</f>
+        <v>21.75</v>
+      </c>
+      <c r="J17" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>21.25</v>
+      </c>
+      <c r="K17" s="3">
+        <f t="shared" ref="K17" ca="1" si="26">J17/2+L17/2</f>
+        <v>21.125</v>
+      </c>
+      <c r="L17" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="M17" s="3">
+        <f t="shared" ref="M17" ca="1" si="27">L17/2+N17/2</f>
+        <v>21.375</v>
+      </c>
+      <c r="N17" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>21.75</v>
+      </c>
+      <c r="O17" s="3">
+        <f t="shared" ref="O17" ca="1" si="28">N17/2+P17/2</f>
+        <v>21.75</v>
+      </c>
+      <c r="P17" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>21.75</v>
+      </c>
+      <c r="Q17" s="3"/>
+    </row>
+    <row r="18" spans="1:17">
+      <c r="A18" s="2">
+        <v>5</v>
+      </c>
+      <c r="B18" s="3">
+        <f ca="1">B17/2+B19/2</f>
+        <v>22.125</v>
+      </c>
+      <c r="C18" s="3">
+        <f t="shared" ref="C18" ca="1" si="29">C17/2+C19/2</f>
+        <v>22</v>
+      </c>
+      <c r="D18" s="3">
+        <f t="shared" ref="D18" ca="1" si="30">D17/2+D19/2</f>
+        <v>21.875</v>
+      </c>
+      <c r="E18" s="3">
+        <f t="shared" ref="E18" ca="1" si="31">E17/2+E19/2</f>
+        <v>22</v>
+      </c>
+      <c r="F18" s="3">
+        <f t="shared" ref="F18" ca="1" si="32">F17/2+F19/2</f>
+        <v>22.125</v>
+      </c>
+      <c r="G18" s="3">
+        <f t="shared" ref="G18" ca="1" si="33">G17/2+G19/2</f>
+        <v>22.4375</v>
+      </c>
+      <c r="H18" s="3">
+        <f t="shared" ref="H18" ca="1" si="34">H17/2+H19/2</f>
+        <v>22.75</v>
+      </c>
+      <c r="I18" s="3">
+        <f t="shared" ref="I18" ca="1" si="35">I17/2+I19/2</f>
+        <v>22.6875</v>
+      </c>
+      <c r="J18" s="3">
+        <f t="shared" ref="J18" ca="1" si="36">J17/2+J19/2</f>
+        <v>22.625</v>
+      </c>
+      <c r="K18" s="3">
+        <f t="shared" ref="K18" ca="1" si="37">K17/2+K19/2</f>
+        <v>22.3125</v>
+      </c>
+      <c r="L18" s="3">
+        <f t="shared" ref="L18" ca="1" si="38">L17/2+L19/2</f>
+        <v>22</v>
+      </c>
+      <c r="M18" s="3">
+        <f t="shared" ref="M18" ca="1" si="39">M17/2+M19/2</f>
+        <v>22.0625</v>
+      </c>
+      <c r="N18" s="3">
+        <f t="shared" ref="N18" ca="1" si="40">N17/2+N19/2</f>
+        <v>22.125</v>
+      </c>
+      <c r="O18" s="3">
+        <f t="shared" ref="O18" ca="1" si="41">O17/2+O19/2</f>
+        <v>22.1875</v>
+      </c>
+      <c r="P18" s="3">
+        <f t="shared" ref="P18" ca="1" si="42">P17/2+P19/2</f>
+        <v>22.25</v>
+      </c>
+      <c r="Q18" s="3"/>
+    </row>
+    <row r="19" spans="1:17">
+      <c r="A19" s="2">
+        <v>6</v>
+      </c>
+      <c r="B19" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>21.75</v>
+      </c>
+      <c r="C19" s="3">
+        <f t="shared" ref="C19:E27" ca="1" si="43">B19/2+D19/2</f>
+        <v>22</v>
+      </c>
+      <c r="D19" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>22.25</v>
+      </c>
+      <c r="E19" s="3">
+        <f t="shared" ca="1" si="43"/>
+        <v>22.25</v>
+      </c>
+      <c r="F19" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>22.25</v>
+      </c>
+      <c r="G19" s="3">
+        <f t="shared" ref="G19" ca="1" si="44">F19/2+H19/2</f>
+        <v>22.75</v>
+      </c>
+      <c r="H19" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>23.25</v>
+      </c>
+      <c r="I19" s="3">
+        <f t="shared" ref="I19" ca="1" si="45">H19/2+J19/2</f>
+        <v>23.625</v>
+      </c>
+      <c r="J19" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="K19" s="3">
+        <f t="shared" ref="K19" ca="1" si="46">J19/2+L19/2</f>
+        <v>23.5</v>
+      </c>
+      <c r="L19" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="M19" s="3">
+        <f t="shared" ref="M19" ca="1" si="47">L19/2+N19/2</f>
+        <v>22.75</v>
+      </c>
+      <c r="N19" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>22.5</v>
+      </c>
+      <c r="O19" s="3">
+        <f t="shared" ref="O19" ca="1" si="48">N19/2+P19/2</f>
+        <v>22.625</v>
+      </c>
+      <c r="P19" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>22.75</v>
+      </c>
+      <c r="Q19" s="3"/>
+    </row>
+    <row r="20" spans="1:17">
+      <c r="A20" s="2">
+        <v>7</v>
+      </c>
+      <c r="B20" s="3">
+        <f ca="1">B19/2+B21/2</f>
+        <v>21.75</v>
+      </c>
+      <c r="C20" s="3">
+        <f t="shared" ref="C20" ca="1" si="49">C19/2+C21/2</f>
+        <v>21.8125</v>
+      </c>
+      <c r="D20" s="3">
+        <f t="shared" ref="D20" ca="1" si="50">D19/2+D21/2</f>
+        <v>21.875</v>
+      </c>
+      <c r="E20" s="3">
+        <f t="shared" ref="E20" ca="1" si="51">E19/2+E21/2</f>
+        <v>21.9375</v>
+      </c>
+      <c r="F20" s="3">
+        <f t="shared" ref="F20" ca="1" si="52">F19/2+F21/2</f>
+        <v>22</v>
+      </c>
+      <c r="G20" s="3">
+        <f t="shared" ref="G20" ca="1" si="53">G19/2+G21/2</f>
+        <v>23.625</v>
+      </c>
+      <c r="H20" s="3">
+        <f t="shared" ref="H20" ca="1" si="54">H19/2+H21/2</f>
+        <v>25.25</v>
+      </c>
+      <c r="I20" s="3">
+        <f t="shared" ref="I20" ca="1" si="55">I19/2+I21/2</f>
+        <v>25.8125</v>
+      </c>
+      <c r="J20" s="3">
+        <f t="shared" ref="J20" ca="1" si="56">J19/2+J21/2</f>
+        <v>26.375</v>
+      </c>
+      <c r="K20" s="3">
+        <f t="shared" ref="K20" ca="1" si="57">K19/2+K21/2</f>
+        <v>26.25</v>
+      </c>
+      <c r="L20" s="3">
+        <f t="shared" ref="L20" ca="1" si="58">L19/2+L21/2</f>
+        <v>26.125</v>
+      </c>
+      <c r="M20" s="3">
+        <f t="shared" ref="M20" ca="1" si="59">M19/2+M21/2</f>
+        <v>26</v>
+      </c>
+      <c r="N20" s="3">
+        <f t="shared" ref="N20" ca="1" si="60">N19/2+N21/2</f>
+        <v>25.875</v>
+      </c>
+      <c r="O20" s="3">
+        <f t="shared" ref="O20" ca="1" si="61">O19/2+O21/2</f>
+        <v>26</v>
+      </c>
+      <c r="P20" s="3">
+        <f t="shared" ref="P20" ca="1" si="62">P19/2+P21/2</f>
+        <v>26.125</v>
+      </c>
+      <c r="Q20" s="3"/>
+    </row>
+    <row r="21" spans="1:17">
+      <c r="A21" s="2">
+        <v>8</v>
+      </c>
+      <c r="B21" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>21.75</v>
+      </c>
+      <c r="C21" s="3">
+        <f t="shared" ref="C21:E21" ca="1" si="63">B21/2+D21/2</f>
+        <v>21.625</v>
+      </c>
+      <c r="D21" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>21.5</v>
+      </c>
+      <c r="E21" s="3">
+        <f t="shared" ca="1" si="63"/>
+        <v>21.625</v>
+      </c>
+      <c r="F21" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>21.75</v>
+      </c>
+      <c r="G21" s="3">
+        <f t="shared" ref="G21" ca="1" si="64">F21/2+H21/2</f>
+        <v>24.5</v>
+      </c>
+      <c r="H21" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>27.25</v>
+      </c>
+      <c r="I21" s="3">
+        <f t="shared" ref="I21" ca="1" si="65">H21/2+J21/2</f>
+        <v>28</v>
+      </c>
+      <c r="J21" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>28.75</v>
+      </c>
+      <c r="K21" s="3">
+        <f t="shared" ref="K21" ca="1" si="66">J21/2+L21/2</f>
+        <v>29</v>
+      </c>
+      <c r="L21" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>29.25</v>
+      </c>
+      <c r="M21" s="3">
+        <f t="shared" ref="M21" ca="1" si="67">L21/2+N21/2</f>
+        <v>29.25</v>
+      </c>
+      <c r="N21" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>29.25</v>
+      </c>
+      <c r="O21" s="3">
+        <f t="shared" ref="O21" ca="1" si="68">N21/2+P21/2</f>
+        <v>29.375</v>
+      </c>
+      <c r="P21" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>29.5</v>
+      </c>
+      <c r="Q21" s="3"/>
+    </row>
+    <row r="22" spans="1:17">
+      <c r="A22" s="2">
+        <v>9</v>
+      </c>
+      <c r="B22" s="3">
+        <f ca="1">B21/2+B23/2</f>
+        <v>21.875</v>
+      </c>
+      <c r="C22" s="3">
+        <f t="shared" ref="C22" ca="1" si="69">C21/2+C23/2</f>
+        <v>21.5625</v>
+      </c>
+      <c r="D22" s="3">
+        <f t="shared" ref="D22" ca="1" si="70">D21/2+D23/2</f>
+        <v>21.25</v>
+      </c>
+      <c r="E22" s="3">
+        <f t="shared" ref="E22" ca="1" si="71">E21/2+E23/2</f>
+        <v>21.375</v>
+      </c>
+      <c r="F22" s="3">
+        <f t="shared" ref="F22" ca="1" si="72">F21/2+F23/2</f>
+        <v>21.5</v>
+      </c>
+      <c r="G22" s="3">
+        <f t="shared" ref="G22" ca="1" si="73">G21/2+G23/2</f>
+        <v>23.1875</v>
+      </c>
+      <c r="H22" s="3">
+        <f t="shared" ref="H22" ca="1" si="74">H21/2+H23/2</f>
+        <v>24.875</v>
+      </c>
+      <c r="I22" s="3">
+        <f t="shared" ref="I22" ca="1" si="75">I21/2+I23/2</f>
+        <v>25.6875</v>
+      </c>
+      <c r="J22" s="3">
+        <f t="shared" ref="J22" ca="1" si="76">J21/2+J23/2</f>
+        <v>26.5</v>
+      </c>
+      <c r="K22" s="3">
+        <f t="shared" ref="K22" ca="1" si="77">K21/2+K23/2</f>
+        <v>26.75</v>
+      </c>
+      <c r="L22" s="3">
+        <f t="shared" ref="L22" ca="1" si="78">L21/2+L23/2</f>
+        <v>27</v>
+      </c>
+      <c r="M22" s="3">
+        <f t="shared" ref="M22" ca="1" si="79">M21/2+M23/2</f>
+        <v>27.1875</v>
+      </c>
+      <c r="N22" s="3">
+        <f t="shared" ref="N22" ca="1" si="80">N21/2+N23/2</f>
+        <v>27.375</v>
+      </c>
+      <c r="O22" s="3">
+        <f t="shared" ref="O22" ca="1" si="81">O21/2+O23/2</f>
+        <v>27.25</v>
+      </c>
+      <c r="P22" s="3">
+        <f t="shared" ref="P22" ca="1" si="82">P21/2+P23/2</f>
+        <v>27.125</v>
+      </c>
+      <c r="Q22" s="3"/>
+    </row>
+    <row r="23" spans="1:17">
+      <c r="A23" s="2">
+        <v>10</v>
+      </c>
+      <c r="B23" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="C23" s="3">
+        <f t="shared" ca="1" si="43"/>
+        <v>21.5</v>
+      </c>
+      <c r="D23" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="E23" s="3">
+        <f t="shared" ca="1" si="43"/>
+        <v>21.125</v>
+      </c>
+      <c r="F23" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>21.25</v>
+      </c>
+      <c r="G23" s="3">
+        <f t="shared" ref="G23" ca="1" si="83">F23/2+H23/2</f>
+        <v>21.875</v>
+      </c>
+      <c r="H23" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>22.5</v>
+      </c>
+      <c r="I23" s="3">
+        <f t="shared" ref="I23" ca="1" si="84">H23/2+J23/2</f>
+        <v>23.375</v>
+      </c>
+      <c r="J23" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>24.25</v>
+      </c>
+      <c r="K23" s="3">
+        <f t="shared" ref="K23" ca="1" si="85">J23/2+L23/2</f>
+        <v>24.5</v>
+      </c>
+      <c r="L23" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>24.75</v>
+      </c>
+      <c r="M23" s="3">
+        <f t="shared" ref="M23" ca="1" si="86">L23/2+N23/2</f>
+        <v>25.125</v>
+      </c>
+      <c r="N23" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>25.5</v>
+      </c>
+      <c r="O23" s="3">
+        <f t="shared" ref="O23" ca="1" si="87">N23/2+P23/2</f>
+        <v>25.125</v>
+      </c>
+      <c r="P23" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>24.75</v>
+      </c>
+      <c r="Q23" s="3"/>
+    </row>
+    <row r="24" spans="1:17">
+      <c r="A24" s="2">
+        <v>11</v>
+      </c>
+      <c r="B24" s="3">
+        <f ca="1">B23/2+B25/2</f>
+        <v>21.5</v>
+      </c>
+      <c r="C24" s="3">
+        <f t="shared" ref="C24" ca="1" si="88">C23/2+C25/2</f>
+        <v>21.375</v>
+      </c>
+      <c r="D24" s="3">
+        <f t="shared" ref="D24" ca="1" si="89">D23/2+D25/2</f>
+        <v>21.25</v>
+      </c>
+      <c r="E24" s="3">
+        <f t="shared" ref="E24" ca="1" si="90">E23/2+E25/2</f>
+        <v>21.25</v>
+      </c>
+      <c r="F24" s="3">
+        <f t="shared" ref="F24" ca="1" si="91">F23/2+F25/2</f>
+        <v>21.25</v>
+      </c>
+      <c r="G24" s="3">
+        <f t="shared" ref="G24" ca="1" si="92">G23/2+G25/2</f>
+        <v>21.6875</v>
+      </c>
+      <c r="H24" s="3">
+        <f t="shared" ref="H24" ca="1" si="93">H23/2+H25/2</f>
+        <v>22.125</v>
+      </c>
+      <c r="I24" s="3">
+        <f t="shared" ref="I24" ca="1" si="94">I23/2+I25/2</f>
+        <v>22.625</v>
+      </c>
+      <c r="J24" s="3">
+        <f t="shared" ref="J24" ca="1" si="95">J23/2+J25/2</f>
+        <v>23.125</v>
+      </c>
+      <c r="K24" s="3">
+        <f t="shared" ref="K24" ca="1" si="96">K23/2+K25/2</f>
+        <v>23.5</v>
+      </c>
+      <c r="L24" s="3">
+        <f t="shared" ref="L24" ca="1" si="97">L23/2+L25/2</f>
+        <v>23.875</v>
+      </c>
+      <c r="M24" s="3">
+        <f t="shared" ref="M24" ca="1" si="98">M23/2+M25/2</f>
+        <v>24.1875</v>
+      </c>
+      <c r="N24" s="3">
+        <f t="shared" ref="N24" ca="1" si="99">N23/2+N25/2</f>
+        <v>24.5</v>
+      </c>
+      <c r="O24" s="3">
+        <f t="shared" ref="O24" ca="1" si="100">O23/2+O25/2</f>
+        <v>24.3125</v>
+      </c>
+      <c r="P24" s="3">
+        <f t="shared" ref="P24" ca="1" si="101">P23/2+P25/2</f>
+        <v>24.125</v>
+      </c>
+      <c r="Q24" s="3"/>
+    </row>
+    <row r="25" spans="1:17">
+      <c r="A25" s="2">
+        <v>12</v>
+      </c>
+      <c r="B25" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="C25" s="3">
+        <f t="shared" ref="C25:E25" ca="1" si="102">B25/2+D25/2</f>
+        <v>21.25</v>
+      </c>
+      <c r="D25" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>21.5</v>
+      </c>
+      <c r="E25" s="3">
+        <f t="shared" ca="1" si="102"/>
+        <v>21.375</v>
+      </c>
+      <c r="F25" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>21.25</v>
+      </c>
+      <c r="G25" s="3">
+        <f t="shared" ref="G25" ca="1" si="103">F25/2+H25/2</f>
+        <v>21.5</v>
+      </c>
+      <c r="H25" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>21.75</v>
+      </c>
+      <c r="I25" s="3">
+        <f t="shared" ref="I25" ca="1" si="104">H25/2+J25/2</f>
+        <v>21.875</v>
+      </c>
+      <c r="J25" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="K25" s="3">
+        <f t="shared" ref="K25" ca="1" si="105">J25/2+L25/2</f>
+        <v>22.5</v>
+      </c>
+      <c r="L25" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="M25" s="3">
+        <f t="shared" ref="M25" ca="1" si="106">L25/2+N25/2</f>
+        <v>23.25</v>
+      </c>
+      <c r="N25" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>23.5</v>
+      </c>
+      <c r="O25" s="3">
+        <f t="shared" ref="O25" ca="1" si="107">N25/2+P25/2</f>
+        <v>23.5</v>
+      </c>
+      <c r="P25" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>23.5</v>
+      </c>
+      <c r="Q25" s="3"/>
+    </row>
+    <row r="26" spans="1:17">
+      <c r="A26" s="2">
+        <v>13</v>
+      </c>
+      <c r="B26" s="3">
+        <f ca="1">B25/2+B27/2</f>
+        <v>21.125</v>
+      </c>
+      <c r="C26" s="3">
+        <f t="shared" ref="C26" ca="1" si="108">C25/2+C27/2</f>
+        <v>21.25</v>
+      </c>
+      <c r="D26" s="3">
+        <f t="shared" ref="D26" ca="1" si="109">D25/2+D27/2</f>
+        <v>21.375</v>
+      </c>
+      <c r="E26" s="3">
+        <f t="shared" ref="E26" ca="1" si="110">E25/2+E27/2</f>
+        <v>21.375</v>
+      </c>
+      <c r="F26" s="3">
+        <f t="shared" ref="F26" ca="1" si="111">F25/2+F27/2</f>
+        <v>21.375</v>
+      </c>
+      <c r="G26" s="3">
+        <f t="shared" ref="G26" ca="1" si="112">G25/2+G27/2</f>
+        <v>21.6875</v>
+      </c>
+      <c r="H26" s="3">
+        <f t="shared" ref="H26" ca="1" si="113">H25/2+H27/2</f>
+        <v>22</v>
+      </c>
+      <c r="I26" s="3">
+        <f t="shared" ref="I26" ca="1" si="114">I25/2+I27/2</f>
+        <v>22.0625</v>
+      </c>
+      <c r="J26" s="3">
+        <f t="shared" ref="J26" ca="1" si="115">J25/2+J27/2</f>
+        <v>22.125</v>
+      </c>
+      <c r="K26" s="3">
+        <f t="shared" ref="K26" ca="1" si="116">K25/2+K27/2</f>
+        <v>22.375</v>
+      </c>
+      <c r="L26" s="3">
+        <f t="shared" ref="L26" ca="1" si="117">L25/2+L27/2</f>
+        <v>22.625</v>
+      </c>
+      <c r="M26" s="3">
+        <f t="shared" ref="M26" ca="1" si="118">M25/2+M27/2</f>
+        <v>22.9375</v>
+      </c>
+      <c r="N26" s="3">
+        <f t="shared" ref="N26" ca="1" si="119">N25/2+N27/2</f>
+        <v>23.25</v>
+      </c>
+      <c r="O26" s="3">
+        <f t="shared" ref="O26" ca="1" si="120">O25/2+O27/2</f>
+        <v>23.3125</v>
+      </c>
+      <c r="P26" s="3">
+        <f t="shared" ref="P26" ca="1" si="121">P25/2+P27/2</f>
+        <v>23.375</v>
+      </c>
+      <c r="Q26" s="3"/>
+    </row>
+    <row r="27" spans="1:17">
+      <c r="A27" s="2">
+        <v>14</v>
+      </c>
+      <c r="B27" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>21.25</v>
+      </c>
+      <c r="C27" s="3">
+        <f t="shared" ca="1" si="43"/>
+        <v>21.25</v>
+      </c>
+      <c r="D27" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>21.25</v>
+      </c>
+      <c r="E27" s="3">
+        <f t="shared" ca="1" si="43"/>
+        <v>21.375</v>
+      </c>
+      <c r="F27" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>21.5</v>
+      </c>
+      <c r="G27" s="3">
+        <f t="shared" ref="G27" ca="1" si="122">F27/2+H27/2</f>
+        <v>21.875</v>
+      </c>
+      <c r="H27" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>22.25</v>
+      </c>
+      <c r="I27" s="3">
+        <f t="shared" ref="I27" ca="1" si="123">H27/2+J27/2</f>
+        <v>22.25</v>
+      </c>
+      <c r="J27" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>22.25</v>
+      </c>
+      <c r="K27" s="3">
+        <f t="shared" ref="K27" ca="1" si="124">J27/2+L27/2</f>
+        <v>22.25</v>
+      </c>
+      <c r="L27" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>22.25</v>
+      </c>
+      <c r="M27" s="3">
+        <f t="shared" ref="M27" ca="1" si="125">L27/2+N27/2</f>
+        <v>22.625</v>
+      </c>
+      <c r="N27" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="O27" s="3">
+        <f t="shared" ref="O27" ca="1" si="126">N27/2+P27/2</f>
+        <v>23.125</v>
+      </c>
+      <c r="P27" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>23.25</v>
+      </c>
+      <c r="Q27" s="3"/>
+    </row>
+    <row r="28" spans="1:17">
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="3"/>
+      <c r="O28" s="3"/>
+      <c r="P28" s="3"/>
+      <c r="Q28" s="3"/>
+    </row>
+    <row r="31" spans="1:17">
+      <c r="B31" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17">
+      <c r="B32" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2">
+      <c r="B33" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>